<commit_message>
Mantap stock opname udah perfect, tinggal perbaiki metode hitung hpp
</commit_message>
<xml_diff>
--- a/db/ZZZ.xlsx
+++ b/db/ZZZ.xlsx
@@ -1816,9 +1816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>